<commit_message>
incluindo nova simulação com os detectores hibridos
</commit_message>
<xml_diff>
--- a/AMPS2019/figures data/comparisons.xlsx
+++ b/AMPS2019/figures data/comparisons.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A87353-698F-4F41-9B1A-B2CA62F2A4A2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="magnitude" sheetId="1" r:id="rId1"/>
     <sheet name="fase" sheetId="2" r:id="rId2"/>
     <sheet name="ambos" sheetId="3" r:id="rId3"/>
     <sheet name="FE" sheetId="4" r:id="rId4"/>
+    <sheet name="Hybrid all" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="41">
   <si>
     <t>km = 5</t>
   </si>
@@ -125,17 +125,41 @@
   <si>
     <t>phi0 = 0</t>
   </si>
+  <si>
+    <t>KxS = -0.1</t>
+  </si>
+  <si>
+    <t>KaS = 0</t>
+  </si>
+  <si>
+    <t>KxS = -0</t>
+  </si>
+  <si>
+    <t>KaS =10</t>
+  </si>
+  <si>
+    <t>Detector híbrido</t>
+  </si>
+  <si>
+    <t>MAG STEP ONLY</t>
+  </si>
+  <si>
+    <t>PHASE STEP ONLY</t>
+  </si>
+  <si>
+    <t>phi_0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.0E+00"/>
-    <numFmt numFmtId="170" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -153,7 +177,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,6 +193,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -208,31 +250,38 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -252,7 +301,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -291,6 +340,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -316,7 +366,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -412,7 +462,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0AB5-48FD-9B14-48E48CE2539A}"/>
             </c:ext>
@@ -504,7 +554,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0AB5-48FD-9B14-48E48CE2539A}"/>
             </c:ext>
@@ -596,7 +646,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0AB5-48FD-9B14-48E48CE2539A}"/>
             </c:ext>
@@ -688,7 +738,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-0AB5-48FD-9B14-48E48CE2539A}"/>
             </c:ext>
@@ -702,11 +752,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="188088344"/>
-        <c:axId val="188087560"/>
+        <c:axId val="188126576"/>
+        <c:axId val="188127360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="188088344"/>
+        <c:axId val="188126576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -760,15 +810,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188087560"/>
+        <c:crossAx val="188127360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="188087560"/>
+        <c:axId val="188127360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -822,10 +872,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188088344"/>
+        <c:crossAx val="188126576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -839,6 +889,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -864,7 +915,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -894,7 +945,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -906,7 +957,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -949,6 +1000,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -974,7 +1026,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1070,7 +1122,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-23BA-42A0-A5BC-63DBBBEC5986}"/>
             </c:ext>
@@ -1162,7 +1214,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-23BA-42A0-A5BC-63DBBBEC5986}"/>
             </c:ext>
@@ -1254,7 +1306,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-23BA-42A0-A5BC-63DBBBEC5986}"/>
             </c:ext>
@@ -1346,7 +1398,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-23BA-42A0-A5BC-63DBBBEC5986}"/>
             </c:ext>
@@ -1360,11 +1412,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="188089912"/>
-        <c:axId val="185875960"/>
+        <c:axId val="235970280"/>
+        <c:axId val="235970672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="188089912"/>
+        <c:axId val="235970280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1418,15 +1470,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="185875960"/>
+        <c:crossAx val="235970672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="185875960"/>
+        <c:axId val="235970672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1480,10 +1532,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188089912"/>
+        <c:crossAx val="235970280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1497,6 +1549,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1522,7 +1575,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1552,7 +1605,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2695,7 +2748,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2731,7 +2784,7 @@
         <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2757,7 +2810,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2795,7 +2848,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2830,23 +2883,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2882,26 +2918,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3074,58 +3093,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R47"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:F37"/>
+      <selection activeCell="B30" sqref="B30:F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
       <c r="H5" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
       <c r="N5" t="s">
         <v>8</v>
       </c>
-      <c r="O5" s="12" t="s">
+      <c r="O5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -3172,7 +3191,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>90</v>
       </c>
@@ -3219,7 +3238,7 @@
         <v>30.4</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <f>B7-15</f>
         <v>75</v>
@@ -3269,7 +3288,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <f t="shared" ref="B9:B13" si="0">B8-15</f>
         <v>60</v>
@@ -3319,7 +3338,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -3369,7 +3388,7 @@
         <v>53.3</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -3419,7 +3438,7 @@
         <v>68.400000000000006</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3469,7 +3488,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3519,39 +3538,39 @@
         <v>70.400000000000006</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
       <c r="H17" t="s">
         <v>7</v>
       </c>
-      <c r="I17" s="12" t="s">
+      <c r="I17" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
       <c r="N17" t="s">
         <v>8</v>
       </c>
-      <c r="O17" s="12" t="s">
+      <c r="O17" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="12"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
@@ -3598,7 +3617,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>90</v>
       </c>
@@ -3645,7 +3664,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <f>B19-15</f>
         <v>75</v>
@@ -3695,7 +3714,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <f t="shared" ref="B21:B25" si="3">B20-15</f>
         <v>60</v>
@@ -3745,7 +3764,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <f t="shared" si="3"/>
         <v>45</v>
@@ -3795,7 +3814,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <f t="shared" si="3"/>
         <v>30</v>
@@ -3845,7 +3864,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <f t="shared" si="3"/>
         <v>15</v>
@@ -3895,7 +3914,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3945,7 +3964,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -3962,39 +3981,39 @@
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2</v>
       </c>
       <c r="B28" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
       <c r="H28" t="s">
         <v>7</v>
       </c>
-      <c r="I28" s="12" t="s">
+      <c r="I28" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="12"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
       <c r="N28" t="s">
         <v>8</v>
       </c>
-      <c r="O28" s="12" t="s">
+      <c r="O28" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="P28" s="12"/>
-      <c r="Q28" s="12"/>
-      <c r="R28" s="12"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P28" s="16"/>
+      <c r="Q28" s="16"/>
+      <c r="R28" s="16"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -4044,7 +4063,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>90</v>
       </c>
@@ -4091,7 +4110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <f>B30-15</f>
         <v>75</v>
@@ -4141,7 +4160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B32" s="1">
         <f t="shared" ref="B32:B36" si="6">B31-15</f>
         <v>60</v>
@@ -4191,7 +4210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B33" s="1">
         <f t="shared" si="6"/>
         <v>45</v>
@@ -4241,7 +4260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
         <f t="shared" si="6"/>
         <v>30</v>
@@ -4291,7 +4310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
         <f t="shared" si="6"/>
         <v>15</v>
@@ -4341,7 +4360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4391,39 +4410,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>9</v>
       </c>
       <c r="B39" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
       <c r="H39" t="s">
         <v>7</v>
       </c>
-      <c r="I39" s="12" t="s">
+      <c r="I39" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="J39" s="12"/>
-      <c r="K39" s="12"/>
-      <c r="L39" s="12"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
       <c r="N39" t="s">
         <v>8</v>
       </c>
-      <c r="O39" s="12" t="s">
+      <c r="O39" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="P39" s="12"/>
-      <c r="Q39" s="12"/>
-      <c r="R39" s="12"/>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P39" s="16"/>
+      <c r="Q39" s="16"/>
+      <c r="R39" s="16"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>6</v>
       </c>
@@ -4470,7 +4489,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
         <v>90</v>
       </c>
@@ -4517,7 +4536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B42" s="1">
         <f>B41-15</f>
         <v>75</v>
@@ -4567,7 +4586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B43" s="1">
         <f t="shared" ref="B43:B47" si="9">B42-15</f>
         <v>60</v>
@@ -4617,7 +4636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B44" s="1">
         <f t="shared" si="9"/>
         <v>45</v>
@@ -4667,7 +4686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B45" s="1">
         <f t="shared" si="9"/>
         <v>30</v>
@@ -4717,7 +4736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B46" s="1">
         <f t="shared" si="9"/>
         <v>15</v>
@@ -4767,7 +4786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B47" s="1">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4819,75 +4838,75 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="I28:L28"/>
+    <mergeCell ref="O28:R28"/>
+    <mergeCell ref="C39:F39"/>
+    <mergeCell ref="I39:L39"/>
+    <mergeCell ref="O39:R39"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="I5:L5"/>
     <mergeCell ref="O5:R5"/>
     <mergeCell ref="I17:L17"/>
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="O17:R17"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="I28:L28"/>
-    <mergeCell ref="O28:R28"/>
-    <mergeCell ref="C39:F39"/>
-    <mergeCell ref="I39:L39"/>
-    <mergeCell ref="O39:R39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R47"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD36"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
       <c r="H5" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
       <c r="N5" t="s">
         <v>8</v>
       </c>
-      <c r="O5" s="12" t="s">
+      <c r="O5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -4934,7 +4953,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>90</v>
       </c>
@@ -4981,7 +5000,7 @@
         <v>69.2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <f>B7-15</f>
         <v>75</v>
@@ -5031,7 +5050,7 @@
         <v>62.7</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <f t="shared" ref="B9:B13" si="0">B8-15</f>
         <v>60</v>
@@ -5081,7 +5100,7 @@
         <v>36.5</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -5131,7 +5150,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -5181,7 +5200,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -5231,7 +5250,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5281,39 +5300,39 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
       <c r="H17" t="s">
         <v>7</v>
       </c>
-      <c r="I17" s="12" t="s">
+      <c r="I17" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
       <c r="N17" t="s">
         <v>8</v>
       </c>
-      <c r="O17" s="12" t="s">
+      <c r="O17" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="12"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
@@ -5360,7 +5379,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>90</v>
       </c>
@@ -5407,7 +5426,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <f>B19-15</f>
         <v>75</v>
@@ -5457,7 +5476,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <f t="shared" ref="B21:B25" si="3">B20-15</f>
         <v>60</v>
@@ -5507,7 +5526,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <f t="shared" si="3"/>
         <v>45</v>
@@ -5557,7 +5576,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <f t="shared" si="3"/>
         <v>30</v>
@@ -5607,7 +5626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <f t="shared" si="3"/>
         <v>15</v>
@@ -5657,7 +5676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5707,7 +5726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -5724,39 +5743,39 @@
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
     </row>
-    <row r="28" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
       <c r="H28" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I28" s="13" t="s">
+      <c r="I28" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
       <c r="N28" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O28" s="13" t="s">
+      <c r="O28" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="13"/>
-    </row>
-    <row r="29" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P28" s="17"/>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="17"/>
+    </row>
+    <row r="29" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>6</v>
       </c>
@@ -5803,7 +5822,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5">
         <v>90</v>
       </c>
@@ -5850,7 +5869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="5">
         <f>B30-15</f>
         <v>75</v>
@@ -5900,7 +5919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5">
         <f t="shared" ref="B32:B36" si="6">B31-15</f>
         <v>60</v>
@@ -5950,7 +5969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5">
         <f t="shared" si="6"/>
         <v>45</v>
@@ -6000,7 +6019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5">
         <f t="shared" si="6"/>
         <v>30</v>
@@ -6050,7 +6069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5">
         <f t="shared" si="6"/>
         <v>15</v>
@@ -6100,7 +6119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -6150,39 +6169,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
       <c r="B39" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
       <c r="H39" t="s">
         <v>7</v>
       </c>
-      <c r="I39" s="12" t="s">
+      <c r="I39" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="J39" s="12"/>
-      <c r="K39" s="12"/>
-      <c r="L39" s="12"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
       <c r="N39" t="s">
         <v>8</v>
       </c>
-      <c r="O39" s="12" t="s">
+      <c r="O39" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="P39" s="12"/>
-      <c r="Q39" s="12"/>
-      <c r="R39" s="12"/>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P39" s="16"/>
+      <c r="Q39" s="16"/>
+      <c r="R39" s="16"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>6</v>
       </c>
@@ -6229,7 +6248,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
         <v>90</v>
       </c>
@@ -6276,7 +6295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B42" s="1">
         <f>B41-15</f>
         <v>75</v>
@@ -6326,7 +6345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B43" s="1">
         <f t="shared" ref="B43:B47" si="9">B42-15</f>
         <v>60</v>
@@ -6376,7 +6395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B44" s="1">
         <f t="shared" si="9"/>
         <v>45</v>
@@ -6426,7 +6445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B45" s="1">
         <f t="shared" si="9"/>
         <v>30</v>
@@ -6476,7 +6495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B46" s="1">
         <f t="shared" si="9"/>
         <v>15</v>
@@ -6526,7 +6545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B47" s="1">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -6578,70 +6597,70 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="I28:L28"/>
+    <mergeCell ref="O28:R28"/>
+    <mergeCell ref="C39:F39"/>
+    <mergeCell ref="I39:L39"/>
+    <mergeCell ref="O39:R39"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="I5:L5"/>
     <mergeCell ref="O5:R5"/>
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="I17:L17"/>
     <mergeCell ref="O17:R17"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="I28:L28"/>
-    <mergeCell ref="O28:R28"/>
-    <mergeCell ref="C39:F39"/>
-    <mergeCell ref="I39:L39"/>
-    <mergeCell ref="O39:R39"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
       <c r="H6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
       <c r="N6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="13" t="s">
+      <c r="O6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-    </row>
-    <row r="7" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+    </row>
+    <row r="7" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
@@ -6688,7 +6707,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>90</v>
       </c>
@@ -6735,7 +6754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <f>B8-15</f>
         <v>75</v>
@@ -6785,7 +6804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <f t="shared" ref="B10:B14" si="0">B9-15</f>
         <v>60</v>
@@ -6835,7 +6854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -6885,7 +6904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -6935,7 +6954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -6985,7 +7004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7046,27 +7065,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="12" max="18" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>20</v>
       </c>
@@ -7081,7 +7100,7 @@
       <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
@@ -7091,7 +7110,7 @@
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1</v>
       </c>
@@ -7120,7 +7139,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>60</v>
       </c>
@@ -7179,14 +7198,14 @@
       <c r="T6" t="s">
         <v>26</v>
       </c>
-      <c r="U6" s="16">
+      <c r="U6" s="14">
         <v>57.44</v>
       </c>
       <c r="V6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>16</v>
       </c>
@@ -7214,40 +7233,40 @@
       <c r="K7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7" s="13">
         <v>-2.4418285516719602E-4</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M7" s="13">
         <v>-3.0778591887778699E-4</v>
       </c>
-      <c r="N7" s="15">
+      <c r="N7" s="13">
         <v>-3.8560076352526601E-4</v>
       </c>
-      <c r="O7" s="15">
+      <c r="O7" s="13">
         <v>-4.51549091744905E-4</v>
       </c>
-      <c r="P7" s="15">
+      <c r="P7" s="13">
         <v>-4.8150479480212202E-4</v>
       </c>
-      <c r="Q7" s="15">
+      <c r="Q7" s="13">
         <v>-5.10724267628524E-4</v>
       </c>
-      <c r="R7" s="15">
+      <c r="R7" s="13">
         <v>-4.9788789751207705E-4</v>
       </c>
-      <c r="T7" s="14">
+      <c r="T7" s="12">
         <v>-4.3612000000000002E-4</v>
       </c>
-      <c r="U7" s="14">
+      <c r="U7" s="12">
         <f>M7</f>
         <v>-3.0778591887778699E-4</v>
       </c>
-      <c r="V7" s="14">
+      <c r="V7" s="12">
         <f>T7-U7</f>
         <v>-1.2833408112221303E-4</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>23</v>
       </c>
@@ -7275,29 +7294,29 @@
       <c r="K8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="15">
+      <c r="L8" s="13">
         <v>3.1592476594434802E-4</v>
       </c>
-      <c r="M8" s="15">
+      <c r="M8" s="13">
         <v>4.7449025019973202E-4</v>
       </c>
-      <c r="N8" s="15">
+      <c r="N8" s="13">
         <v>7.7239781160635501E-4</v>
       </c>
-      <c r="O8" s="15">
+      <c r="O8" s="13">
         <v>1.3117119783633299E-3</v>
       </c>
-      <c r="P8" s="15">
+      <c r="P8" s="13">
         <v>2.28980234913074E-3</v>
       </c>
-      <c r="Q8" s="15">
+      <c r="Q8" s="13">
         <v>4.0365862613823897E-3</v>
       </c>
-      <c r="R8" s="15">
+      <c r="R8" s="13">
         <v>7.1247945485558304E-3</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -7306,15 +7325,15 @@
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="K9" s="10"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-    </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>2</v>
       </c>
@@ -7332,15 +7351,15 @@
       <c r="K10" s="10">
         <v>2</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="L10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
       <c r="T10" t="s">
         <v>25</v>
       </c>
@@ -7348,7 +7367,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>60</v>
       </c>
@@ -7407,14 +7426,14 @@
       <c r="T11" t="s">
         <v>26</v>
       </c>
-      <c r="U11" s="16">
+      <c r="U11" s="14">
         <v>53.883099999999999</v>
       </c>
       <c r="V11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>16</v>
       </c>
@@ -7442,40 +7461,40 @@
       <c r="K12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="L12" s="15">
+      <c r="L12" s="13">
         <v>9.2209982382471397E-4</v>
       </c>
-      <c r="M12" s="15">
+      <c r="M12" s="13">
         <v>1.1548573225405401E-3</v>
       </c>
-      <c r="N12" s="15">
+      <c r="N12" s="13">
         <v>1.56349386036029E-3</v>
       </c>
-      <c r="O12" s="15">
+      <c r="O12" s="13">
         <v>1.9693845359400899E-3</v>
       </c>
-      <c r="P12" s="15">
+      <c r="P12" s="13">
         <v>2.4217303939699899E-3</v>
       </c>
-      <c r="Q12" s="15">
+      <c r="Q12" s="13">
         <v>2.7540626398422901E-3</v>
       </c>
-      <c r="R12" s="15">
+      <c r="R12" s="13">
         <v>3.3583214962169998E-3</v>
       </c>
-      <c r="T12" s="14">
+      <c r="T12" s="12">
         <v>6.9541000000000004E-4</v>
       </c>
-      <c r="U12" s="14">
+      <c r="U12" s="12">
         <f>M12</f>
         <v>1.1548573225405401E-3</v>
       </c>
-      <c r="V12" s="14">
+      <c r="V12" s="12">
         <f>T12-U12</f>
         <v>-4.5944732254054005E-4</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>23</v>
       </c>
@@ -7503,29 +7522,29 @@
       <c r="K13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="L13" s="15">
+      <c r="L13" s="13">
         <v>5.0775219516712604E-4</v>
       </c>
-      <c r="M13" s="15">
+      <c r="M13" s="13">
         <v>6.6355545857318401E-4</v>
       </c>
-      <c r="N13" s="15">
+      <c r="N13" s="13">
         <v>1.0284187054903299E-3</v>
       </c>
-      <c r="O13" s="15">
+      <c r="O13" s="13">
         <v>1.6047673297552301E-3</v>
       </c>
-      <c r="P13" s="15">
+      <c r="P13" s="13">
         <v>2.5510553421825002E-3</v>
       </c>
-      <c r="Q13" s="15">
+      <c r="Q13" s="13">
         <v>4.1898214189159504E-3</v>
       </c>
-      <c r="R13" s="15">
+      <c r="R13" s="13">
         <v>7.2452191974482398E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -7534,15 +7553,15 @@
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
       <c r="K14" s="10"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-    </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>3</v>
       </c>
@@ -7560,15 +7579,15 @@
       <c r="K15" s="10">
         <v>3</v>
       </c>
-      <c r="L15" s="15" t="s">
+      <c r="L15" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
       <c r="T15" t="s">
         <v>25</v>
       </c>
@@ -7576,7 +7595,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>60</v>
       </c>
@@ -7635,14 +7654,14 @@
       <c r="T16" t="s">
         <v>26</v>
       </c>
-      <c r="U16" s="17">
+      <c r="U16" s="15">
         <v>38.9</v>
       </c>
       <c r="V16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>16</v>
       </c>
@@ -7670,40 +7689,40 @@
       <c r="K17" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="L17" s="15">
+      <c r="L17" s="13">
         <v>4.6706650030491E-4</v>
       </c>
-      <c r="M17" s="15">
+      <c r="M17" s="13">
         <v>6.3362835188788798E-4</v>
       </c>
-      <c r="N17" s="15">
+      <c r="N17" s="13">
         <v>8.8422796159014802E-4</v>
       </c>
-      <c r="O17" s="15">
+      <c r="O17" s="13">
         <v>1.1804504785950401E-3</v>
       </c>
-      <c r="P17" s="15">
+      <c r="P17" s="13">
         <v>1.53628650276499E-3</v>
       </c>
-      <c r="Q17" s="15">
+      <c r="Q17" s="13">
         <v>1.8599487396029201E-3</v>
       </c>
-      <c r="R17" s="15">
+      <c r="R17" s="13">
         <v>2.5360260889802999E-3</v>
       </c>
-      <c r="T17" s="14">
+      <c r="T17" s="12">
         <v>9.5219E-4</v>
       </c>
-      <c r="U17" s="14">
+      <c r="U17" s="12">
         <f>P17</f>
         <v>1.53628650276499E-3</v>
       </c>
-      <c r="V17" s="14">
+      <c r="V17" s="12">
         <f>T17-U17</f>
         <v>-5.8409650276499E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>23</v>
       </c>
@@ -7731,29 +7750,29 @@
       <c r="K18" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="L18" s="15">
+      <c r="L18" s="13">
         <v>3.66822236813724E-4</v>
       </c>
-      <c r="M18" s="15">
+      <c r="M18" s="13">
         <v>5.0812281651283105E-4</v>
       </c>
-      <c r="N18" s="15">
+      <c r="N18" s="13">
         <v>8.2946618387239599E-4</v>
       </c>
-      <c r="O18" s="15">
+      <c r="O18" s="13">
         <v>1.3980287332269999E-3</v>
       </c>
-      <c r="P18" s="15">
+      <c r="P18" s="13">
         <v>2.41956148991253E-3</v>
       </c>
-      <c r="Q18" s="15">
+      <c r="Q18" s="13">
         <v>4.1148268401237399E-3</v>
       </c>
-      <c r="R18" s="15">
+      <c r="R18" s="13">
         <v>7.2515164053988303E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -7770,23 +7789,23 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
       <c r="Q23">
         <v>1</v>
       </c>
       <c r="R23">
         <v>1</v>
       </c>
-      <c r="S23" s="14">
+      <c r="S23" s="12">
         <f>T7</f>
         <v>-4.3612000000000002E-4</v>
       </c>
@@ -7794,7 +7813,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -7816,7 +7835,7 @@
       <c r="R24">
         <v>0</v>
       </c>
-      <c r="S24" s="14">
+      <c r="S24" s="12">
         <f>T12</f>
         <v>6.9541000000000004E-4</v>
       </c>
@@ -7824,7 +7843,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>90</v>
       </c>
@@ -7846,7 +7865,7 @@
       <c r="R25">
         <v>1</v>
       </c>
-      <c r="S25" s="14">
+      <c r="S25" s="12">
         <f>T17</f>
         <v>9.5219E-4</v>
       </c>
@@ -7854,7 +7873,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f>A25-15</f>
         <v>75</v>
@@ -7872,7 +7891,7 @@
         <v>4.5613712777088896E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f t="shared" ref="A27:A31" si="6">A26-15</f>
         <v>60</v>
@@ -7890,7 +7909,7 @@
         <v>3.8977317570133602E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f t="shared" si="6"/>
         <v>45</v>
@@ -7908,7 +7927,7 @@
         <v>3.2975059668812002E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f t="shared" si="6"/>
         <v>30</v>
@@ -7926,7 +7945,7 @@
         <v>2.5331651692455698E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f t="shared" si="6"/>
         <v>15</v>
@@ -7944,7 +7963,7 @@
         <v>1.9489734398989E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -7962,18 +7981,18 @@
         <v>1.6553587277590199E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>6</v>
       </c>
@@ -7990,7 +8009,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>90</v>
       </c>
@@ -8007,7 +8026,7 @@
         <v>7.0574809634244501E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <f>A36-15</f>
         <v>75</v>
@@ -8025,7 +8044,7 @@
         <v>7.2041053429457904E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <f t="shared" ref="A38:A42" si="7">A37-15</f>
         <v>60</v>
@@ -8043,7 +8062,7 @@
         <v>7.0858903571889599E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <f t="shared" si="7"/>
         <v>45</v>
@@ -8061,7 +8080,7 @@
         <v>7.1479880564852098E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <f t="shared" si="7"/>
         <v>30</v>
@@ -8079,7 +8098,7 @@
         <v>7.0872673458018901E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <f t="shared" si="7"/>
         <v>15</v>
@@ -8097,7 +8116,7 @@
         <v>7.05196901451032E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -8123,4 +8142,800 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="I4" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="1">
+        <v>60</v>
+      </c>
+      <c r="D5" s="1">
+        <v>50</v>
+      </c>
+      <c r="E5" s="1">
+        <v>40</v>
+      </c>
+      <c r="F5" s="1">
+        <v>30</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="1">
+        <v>60</v>
+      </c>
+      <c r="J5" s="1">
+        <v>50</v>
+      </c>
+      <c r="K5" s="1">
+        <v>40</v>
+      </c>
+      <c r="L5" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="20">
+        <v>0</v>
+      </c>
+      <c r="D6" s="20">
+        <v>0</v>
+      </c>
+      <c r="E6" s="20">
+        <v>0</v>
+      </c>
+      <c r="F6" s="21">
+        <v>41.41</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="20">
+        <v>0</v>
+      </c>
+      <c r="J6" s="20">
+        <v>0</v>
+      </c>
+      <c r="K6" s="20">
+        <v>0</v>
+      </c>
+      <c r="L6" s="20">
+        <v>33.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <f>+B6+15</f>
+        <v>15</v>
+      </c>
+      <c r="C7" s="20">
+        <v>0</v>
+      </c>
+      <c r="D7" s="20">
+        <v>0</v>
+      </c>
+      <c r="E7" s="20">
+        <v>0</v>
+      </c>
+      <c r="F7" s="21">
+        <v>40.64</v>
+      </c>
+      <c r="H7" s="1">
+        <f>+H6+15</f>
+        <v>15</v>
+      </c>
+      <c r="I7" s="20">
+        <v>0</v>
+      </c>
+      <c r="J7" s="20">
+        <v>0</v>
+      </c>
+      <c r="K7" s="20">
+        <v>0</v>
+      </c>
+      <c r="L7" s="20">
+        <v>34.96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <f t="shared" ref="B8:B12" si="0">+B7+15</f>
+        <v>30</v>
+      </c>
+      <c r="C8" s="20">
+        <v>0</v>
+      </c>
+      <c r="D8" s="20">
+        <v>0</v>
+      </c>
+      <c r="E8" s="20">
+        <v>0</v>
+      </c>
+      <c r="F8" s="21">
+        <v>49.47</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" ref="H8:H12" si="1">+H7+15</f>
+        <v>30</v>
+      </c>
+      <c r="I8" s="20">
+        <v>0</v>
+      </c>
+      <c r="J8" s="20">
+        <v>0</v>
+      </c>
+      <c r="K8" s="20">
+        <v>0</v>
+      </c>
+      <c r="L8" s="20">
+        <v>44.48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="C9" s="20">
+        <v>0</v>
+      </c>
+      <c r="D9" s="20">
+        <v>0</v>
+      </c>
+      <c r="E9" s="20">
+        <v>0</v>
+      </c>
+      <c r="F9" s="21">
+        <v>67.89</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="I9" s="20">
+        <v>0</v>
+      </c>
+      <c r="J9" s="20">
+        <v>0</v>
+      </c>
+      <c r="K9" s="20">
+        <v>0.01</v>
+      </c>
+      <c r="L9" s="20">
+        <v>63.12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="C10" s="20">
+        <v>0</v>
+      </c>
+      <c r="D10" s="20">
+        <v>0</v>
+      </c>
+      <c r="E10" s="20">
+        <v>1.19</v>
+      </c>
+      <c r="F10" s="21">
+        <v>87.12</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="I10" s="20">
+        <v>0</v>
+      </c>
+      <c r="J10" s="20">
+        <v>0</v>
+      </c>
+      <c r="K10" s="20">
+        <v>1.04</v>
+      </c>
+      <c r="L10" s="20">
+        <v>85.92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="C11" s="20">
+        <v>0</v>
+      </c>
+      <c r="D11" s="20">
+        <v>0.06</v>
+      </c>
+      <c r="E11" s="21">
+        <v>34.31</v>
+      </c>
+      <c r="F11" s="20">
+        <v>96.79</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="I11" s="20">
+        <v>0</v>
+      </c>
+      <c r="J11" s="20">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K11" s="20">
+        <v>32.229999999999997</v>
+      </c>
+      <c r="L11" s="20">
+        <v>96.54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="C12" s="20">
+        <v>0.01</v>
+      </c>
+      <c r="D12" s="21">
+        <v>14.78</v>
+      </c>
+      <c r="E12" s="21">
+        <v>91.39</v>
+      </c>
+      <c r="F12" s="20">
+        <v>98.92</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="I12" s="20">
+        <v>0.08</v>
+      </c>
+      <c r="J12" s="20">
+        <v>14.55</v>
+      </c>
+      <c r="K12" s="20">
+        <v>88.31</v>
+      </c>
+      <c r="L12" s="20">
+        <v>98.76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="1">
+        <v>60</v>
+      </c>
+      <c r="D17" s="1">
+        <v>50</v>
+      </c>
+      <c r="E17" s="1">
+        <v>40</v>
+      </c>
+      <c r="F17" s="1">
+        <v>30</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="1">
+        <v>60</v>
+      </c>
+      <c r="J17" s="1">
+        <v>50</v>
+      </c>
+      <c r="K17" s="1">
+        <v>40</v>
+      </c>
+      <c r="L17" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="20">
+        <v>0</v>
+      </c>
+      <c r="D18" s="20">
+        <v>0.17</v>
+      </c>
+      <c r="E18" s="21">
+        <v>56.76</v>
+      </c>
+      <c r="F18" s="20">
+        <v>97.57</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="20">
+        <v>0</v>
+      </c>
+      <c r="J18" s="20">
+        <v>0.17</v>
+      </c>
+      <c r="K18" s="22">
+        <v>86.21</v>
+      </c>
+      <c r="L18" s="20">
+        <v>99.04</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <f>+B18+15</f>
+        <v>15</v>
+      </c>
+      <c r="C19" s="20">
+        <v>0</v>
+      </c>
+      <c r="D19" s="20">
+        <v>0</v>
+      </c>
+      <c r="E19" s="20">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F19" s="21">
+        <v>84.28</v>
+      </c>
+      <c r="H19" s="1">
+        <f>+H18+15</f>
+        <v>15</v>
+      </c>
+      <c r="I19" s="20">
+        <v>0</v>
+      </c>
+      <c r="J19" s="20">
+        <v>0</v>
+      </c>
+      <c r="K19" s="21">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="L19" s="22">
+        <v>90.29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <f t="shared" ref="B20:B24" si="2">+B19+15</f>
+        <v>30</v>
+      </c>
+      <c r="C20" s="20">
+        <v>0</v>
+      </c>
+      <c r="D20" s="20">
+        <v>0</v>
+      </c>
+      <c r="E20" s="20">
+        <v>0</v>
+      </c>
+      <c r="F20" s="21">
+        <v>43.48</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" ref="H20:H24" si="3">+H19+15</f>
+        <v>30</v>
+      </c>
+      <c r="I20" s="20">
+        <v>0</v>
+      </c>
+      <c r="J20" s="20">
+        <v>0</v>
+      </c>
+      <c r="K20" s="20">
+        <v>0</v>
+      </c>
+      <c r="L20" s="22">
+        <v>56.38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="C21" s="20">
+        <v>0</v>
+      </c>
+      <c r="D21" s="20">
+        <v>0</v>
+      </c>
+      <c r="E21" s="20">
+        <v>0</v>
+      </c>
+      <c r="F21" s="21">
+        <v>13.77</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="I21" s="20">
+        <v>0</v>
+      </c>
+      <c r="J21" s="20">
+        <v>0</v>
+      </c>
+      <c r="K21" s="20">
+        <v>0</v>
+      </c>
+      <c r="L21" s="22">
+        <v>24.34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="C22" s="20">
+        <v>0</v>
+      </c>
+      <c r="D22" s="20">
+        <v>0</v>
+      </c>
+      <c r="E22" s="20">
+        <v>0</v>
+      </c>
+      <c r="F22" s="21">
+        <v>5.22</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="I22" s="20">
+        <v>0</v>
+      </c>
+      <c r="J22" s="20">
+        <v>0</v>
+      </c>
+      <c r="K22" s="20">
+        <v>0</v>
+      </c>
+      <c r="L22" s="22">
+        <v>17.55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="C23" s="20">
+        <v>0</v>
+      </c>
+      <c r="D23" s="20">
+        <v>0</v>
+      </c>
+      <c r="E23" s="20">
+        <v>0</v>
+      </c>
+      <c r="F23" s="21">
+        <v>3.62</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+      <c r="I23" s="20">
+        <v>0</v>
+      </c>
+      <c r="J23" s="20">
+        <v>0</v>
+      </c>
+      <c r="K23" s="20">
+        <v>0.86</v>
+      </c>
+      <c r="L23" s="22">
+        <v>24.41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="C24" s="20">
+        <v>0</v>
+      </c>
+      <c r="D24" s="20">
+        <v>0</v>
+      </c>
+      <c r="E24" s="20">
+        <v>0</v>
+      </c>
+      <c r="F24" s="21">
+        <v>2.65</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
+      <c r="I24" s="20">
+        <v>0</v>
+      </c>
+      <c r="J24" s="20">
+        <v>0.05</v>
+      </c>
+      <c r="K24" s="20">
+        <v>5.74</v>
+      </c>
+      <c r="L24" s="22">
+        <v>28.48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>60</v>
+      </c>
+      <c r="D31">
+        <v>50</v>
+      </c>
+      <c r="E31">
+        <v>40</v>
+      </c>
+      <c r="F31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32" s="18">
+        <v>0</v>
+      </c>
+      <c r="D32" s="18">
+        <v>0</v>
+      </c>
+      <c r="E32" s="18">
+        <v>0</v>
+      </c>
+      <c r="F32" s="18">
+        <v>28.68</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <f>+B32+15</f>
+        <v>15</v>
+      </c>
+      <c r="C33" s="18">
+        <v>0</v>
+      </c>
+      <c r="D33" s="18">
+        <v>0</v>
+      </c>
+      <c r="E33" s="18">
+        <v>0</v>
+      </c>
+      <c r="F33" s="18">
+        <v>3.83</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <f t="shared" ref="B34:B38" si="4">+B33+15</f>
+        <v>30</v>
+      </c>
+      <c r="C34" s="18">
+        <v>0</v>
+      </c>
+      <c r="D34" s="18">
+        <v>0</v>
+      </c>
+      <c r="E34" s="18">
+        <v>0</v>
+      </c>
+      <c r="F34" s="18">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="C35" s="18">
+        <v>0</v>
+      </c>
+      <c r="D35" s="18">
+        <v>0</v>
+      </c>
+      <c r="E35" s="18">
+        <v>0</v>
+      </c>
+      <c r="F35" s="18">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="C36" s="18">
+        <v>0</v>
+      </c>
+      <c r="D36" s="18">
+        <v>0</v>
+      </c>
+      <c r="E36" s="18">
+        <v>0</v>
+      </c>
+      <c r="F36" s="18">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <f t="shared" si="4"/>
+        <v>75</v>
+      </c>
+      <c r="C37" s="18">
+        <v>0</v>
+      </c>
+      <c r="D37" s="18">
+        <v>0</v>
+      </c>
+      <c r="E37" s="18">
+        <v>0</v>
+      </c>
+      <c r="F37" s="18">
+        <v>4.07</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+      <c r="C38" s="18">
+        <v>0</v>
+      </c>
+      <c r="D38" s="18">
+        <v>0</v>
+      </c>
+      <c r="E38" s="18">
+        <v>0.01</v>
+      </c>
+      <c r="F38" s="18">
+        <v>5.75</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="I16:L16"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>